<commit_message>
Ajouter varia au rapports préliminaire
</commit_message>
<xml_diff>
--- a/Rapport_Preliminaire_TP2.xlsx
+++ b/Rapport_Preliminaire_TP2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LordCatzorz\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LordCatzorz\Documents\GLO-2001-TP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A743297-4CEA-419D-82E3-B7C7C827CACC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA715B61-70A2-406A-A7D9-4AAFDC26125E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2685" yWindow="2685" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -279,7 +279,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>No</t>
   </si>
@@ -468,6 +468,12 @@
   </si>
   <si>
     <t xml:space="preserve"> 111 244 023 - 111 124 564</t>
+  </si>
+  <si>
+    <t>Varia</t>
+  </si>
+  <si>
+    <t>Correction / Révision / Formattage / Packaging</t>
   </si>
 </sst>
 </file>
@@ -967,8 +973,8 @@
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1:S94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1341,9 +1347,15 @@
       <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
+      <c r="A36" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="11">
+        <v>3</v>
+      </c>
       <c r="D36" s="11"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1371,7 +1383,7 @@
       </c>
       <c r="C40" s="6">
         <f>SUM(C8:C39)</f>
-        <v>26.25</v>
+        <v>29.25</v>
       </c>
       <c r="D40" s="6">
         <f>SUM(D8:D39)</f>

</xml_diff>